<commit_message>
Updated excel template, bulk upload only button hidden when permission not granted
</commit_message>
<xml_diff>
--- a/public/downloads/excel/lab_received_template.xlsx
+++ b/public/downloads/excel/lab_received_template.xlsx
@@ -522,13 +522,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="1" hidden="1"/>
   </cols>
   <sheetData>

</xml_diff>